<commit_message>
Update of Event Sorting and Addition of General Log View
</commit_message>
<xml_diff>
--- a/Sorting/Event_Sorting.xlsx
+++ b/Sorting/Event_Sorting.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A141262-D4DC-4F95-8D59-BCC5CAB88AAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2012F86A-DC5F-4442-957E-6EB58B5A0A37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>_event_concept_name_</t>
   </si>
@@ -475,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B3" sqref="B3:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -513,16 +513,16 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B39" si="0">B3+100</f>
+        <f t="shared" ref="B4:B43" si="0">B3+100</f>
         <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -531,7 +531,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -549,7 +549,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -576,7 +576,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -585,7 +585,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -594,7 +594,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -603,7 +603,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -612,7 +612,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -630,7 +630,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -639,7 +639,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -648,7 +648,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -657,7 +657,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -666,7 +666,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -684,7 +684,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -693,7 +693,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -702,7 +702,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -711,7 +711,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -720,7 +720,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
@@ -729,7 +729,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -738,7 +738,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
@@ -747,7 +747,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
@@ -756,7 +756,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
@@ -765,7 +765,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
@@ -783,7 +783,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
@@ -792,7 +792,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -801,7 +801,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
@@ -810,7 +810,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -819,7 +819,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -828,31 +828,47 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>23</v>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>4200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>